<commit_message>
feat: add download directory selection and PDF download functionality in RcelWindow
</commit_message>
<xml_diff>
--- a/ejemplos_api/rcel.xlsx
+++ b/ejemplos_api/rcel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,11 @@
           <t>hasta</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ubicacion_descarga</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -506,6 +511,11 @@
           <t>31/12/2024</t>
         </is>
       </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>./descargas/RCEL/20987654321</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -541,6 +551,11 @@
       <c r="G3" t="inlineStr">
         <is>
           <t>31/12/2024</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>./descargas/RCEL/20999999999</t>
         </is>
       </c>
     </row>

</xml_diff>